<commit_message>
Implement test for error on 2 value preamble
</commit_message>
<xml_diff>
--- a/template_examples/cytof_e4412_analysis_template.xlsx
+++ b/template_examples/cytof_e4412_analysis_template.xlsx
@@ -209,7 +209,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2086" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2085" uniqueCount="49">
   <si>
     <t xml:space="preserve">#title</t>
   </si>
@@ -593,10 +593,10 @@
   <dimension ref="A1:I2009"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C2" activeCellId="0" sqref="C2"/>
+      <selection pane="topLeft" activeCell="D2" activeCellId="0" sqref="D2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.55078125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.5625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="101" min="1" style="0" width="30.7"/>
   </cols>
@@ -618,9 +618,6 @@
         <v>3</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="D2" s="2" t="s">
         <v>4</v>
       </c>
     </row>
@@ -10784,10 +10781,10 @@
   <dimension ref="B1:D16"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="1" sqref="C2 A1"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="1" sqref="D2 A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.55078125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.5625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="101" min="2" style="0" width="30.7"/>
   </cols>
@@ -10967,10 +10964,10 @@
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="1" sqref="C2 A1"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="1" sqref="D2 A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.55078125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.5625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="101" min="2" style="0" width="30.7"/>
   </cols>

</xml_diff>